<commit_message>
fix: actualizar nombres de productos en la galeríaImplementa la actualización de los nombres de productos en los enlaces del top-rowutilizando productManager.getProduct() para obtener la información.Corrige un error donde se buscaba la propiedad 'name' cuando en realidad la propiedad correcta es 'nombre' en el objeto del producto.Además, convierte los nombres de productos a minúsculas para manteneruna visualización consistente en la interfaz de usuario.
</commit_message>
<xml_diff>
--- a/imagenes_drive.xlsx
+++ b/imagenes_drive.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7815" windowHeight="5205"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
   <si>
     <t>nombre</t>
   </si>
@@ -33,6 +33,18 @@
     <t>link_vista</t>
   </si>
   <si>
+    <t>evol0088.png</t>
+  </si>
+  <si>
+    <t>1nfI5VLK3uGqGq2WeJTrgiggCfpxO2nW9</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1nfI5VLK3uGqGq2WeJTrgiggCfpxO2nW9/view?usp=drivesdk</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/uc?export=view&amp;id=1nfI5VLK3uGqGq2WeJTrgiggCfpxO2nW9</t>
+  </si>
+  <si>
     <t>evol1000.png</t>
   </si>
   <si>
@@ -94,15 +106,6 @@
   </si>
   <si>
     <t>evol0088.webp</t>
-  </si>
-  <si>
-    <t>1wU3WSWy2QtVqepB5lBClIlXkK_xWANWB</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1wU3WSWy2QtVqepB5lBClIlXkK_xWANWB/view?usp=drivesdk</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/uc?export=view&amp;id=1wU3WSWy2QtVqepB5lBClIlXkK_xWANWB</t>
   </si>
   <si>
     <t>evol0330.jpg</t>
@@ -406,6 +409,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -753,15 +757,12 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="43.140625" customWidth="1"/>
-    <col min="3" max="3" width="76.7109375" customWidth="1"/>
-    <col min="4" max="4" width="82.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -864,342 +865,341 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D15" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D16" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C17" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D17" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D18" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B19" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C19" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D19" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D20" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C21" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D21" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B22" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C22" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D22" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C23" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D23" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B24" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C24" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D24" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B25" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C25" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D25" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B26" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C26" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D26" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B27" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C27" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D27" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B28" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C28" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D28" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B29" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C29" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D29" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B30" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C30" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D30" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B31" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C31" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D31" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Actualizacion de datso en los json
</commit_message>
<xml_diff>
--- a/imagenes_drive.xlsx
+++ b/imagenes_drive.xlsx
@@ -9,17 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7815" windowHeight="5205"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="145">
   <si>
     <t>nombre</t>
   </si>
@@ -33,6 +33,54 @@
     <t>link_vista</t>
   </si>
   <si>
+    <t>EGWX 01.png</t>
+  </si>
+  <si>
+    <t>1BgwDF-x074YoMMB-mDYESEaqC2f_yOjJ</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1BgwDF-x074YoMMB-mDYESEaqC2f_yOjJ/view?usp=drivesdk</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/uc?export=view&amp;id=1BgwDF-x074YoMMB-mDYESEaqC2f_yOjJ</t>
+  </si>
+  <si>
+    <t>EGWX 02.png</t>
+  </si>
+  <si>
+    <t>1EDLSpqESmqhKp7xv2VUi5tJfPNY87I3H</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1EDLSpqESmqhKp7xv2VUi5tJfPNY87I3H/view?usp=drivesdk</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/uc?export=view&amp;id=1EDLSpqESmqhKp7xv2VUi5tJfPNY87I3H</t>
+  </si>
+  <si>
+    <t>PX120314.png</t>
+  </si>
+  <si>
+    <t>1weDOT_VWkZKZAz4jS8TVZsetiUcvCN9l</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1weDOT_VWkZKZAz4jS8TVZsetiUcvCN9l/view?usp=drivesdk</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/uc?export=view&amp;id=1weDOT_VWkZKZAz4jS8TVZsetiUcvCN9l</t>
+  </si>
+  <si>
+    <t>PROBOT41.png</t>
+  </si>
+  <si>
+    <t>1qrNWZscYLaNY3tjBvyWBCrhyf_YkY9P_</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1qrNWZscYLaNY3tjBvyWBCrhyf_YkY9P_/view?usp=drivesdk</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/uc?export=view&amp;id=1qrNWZscYLaNY3tjBvyWBCrhyf_YkY9P_</t>
+  </si>
+  <si>
     <t>evol0088.png</t>
   </si>
   <si>
@@ -81,6 +129,30 @@
     <t>https://drive.google.com/uc?export=view&amp;id=1WUt0ka-yyFo63FTM49NWDYNDNiO_04gm</t>
   </si>
   <si>
+    <t>GAG12103AR.jpg</t>
+  </si>
+  <si>
+    <t>19PO9oKCI7tFYmwSmls9HncZeKFLKYsHM</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/19PO9oKCI7tFYmwSmls9HncZeKFLKYsHM/view?usp=drivesdk</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/uc?export=view&amp;id=19PO9oKCI7tFYmwSmls9HncZeKFLKYsHM</t>
+  </si>
+  <si>
+    <t>TOR01522.jpg</t>
+  </si>
+  <si>
+    <t>1D6zNN_9DGy0dFt9raoWvefgiUeE2dVYx</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1D6zNN_9DGy0dFt9raoWvefgiUeE2dVYx/view?usp=drivesdk</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/uc?export=view&amp;id=1D6zNN_9DGy0dFt9raoWvefgiUeE2dVYx</t>
+  </si>
+  <si>
     <t>logo-ferremax.png</t>
   </si>
   <si>
@@ -105,9 +177,6 @@
     <t>https://drive.google.com/uc?export=view&amp;id=1KK_TQrE0L6lVvyr8tfVlByktAqgtNhpn</t>
   </si>
   <si>
-    <t>evol0088.webp</t>
-  </si>
-  <si>
     <t>evol0330.jpg</t>
   </si>
   <si>
@@ -216,9 +285,6 @@
     <t>https://drive.google.com/uc?export=view&amp;id=1dXUQ9WsxzAZey_wt6G2mS7N6Li-NJbSV</t>
   </si>
   <si>
-    <t>evorieg153.jpg</t>
-  </si>
-  <si>
     <t>1lKfYjkIwKWP0ylRb7kAHB6MEsxMj5AyG</t>
   </si>
   <si>
@@ -288,15 +354,6 @@
     <t>https://drive.google.com/uc?export=view&amp;id=18PywtpchMGSXpToC9emFelBbnkIO851b</t>
   </si>
   <si>
-    <t>1FZ2sujtzzwh8q9gK9EYWkPQbxd1-_zlu</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1FZ2sujtzzwh8q9gK9EYWkPQbxd1-_zlu/view?usp=drivesdk</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/uc?export=view&amp;id=1FZ2sujtzzwh8q9gK9EYWkPQbxd1-_zlu</t>
-  </si>
-  <si>
     <t>evol3970.jpg</t>
   </si>
   <si>
@@ -391,13 +448,19 @@
   </si>
   <si>
     <t>https://drive.google.com/uc?export=view&amp;id=1OFRhg3wSMFQ6TYNMMxMweX1JIEsXmKdY</t>
+  </si>
+  <si>
+    <t>articulo</t>
+  </si>
+  <si>
+    <t>evorieg0153.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -409,7 +472,13 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -420,7 +489,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -443,15 +512,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -754,18 +838,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="44.28515625" customWidth="1"/>
+    <col min="3" max="3" width="106.7109375" customWidth="1"/>
+    <col min="4" max="4" width="107.140625" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -778,8 +866,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -792,8 +883,12 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="3" t="str">
+        <f>LEFT(A2,FIND(".",A2)-1)</f>
+        <v>EGWX 01</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -806,8 +901,12 @@
       <c r="D3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="3" t="str">
+        <f>LEFT(A3,FIND(".",A3)-1)</f>
+        <v>EGWX 02</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -820,8 +919,12 @@
       <c r="D4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="3" t="str">
+        <f t="shared" ref="E4:E36" si="0">LEFT(A4,FIND(".",A4)-1)</f>
+        <v>PX120314</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -834,8 +937,12 @@
       <c r="D5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PROBOT41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -848,8 +955,12 @@
       <c r="D6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>evol0088</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -862,344 +973,535 @@
       <c r="D7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>evol1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
         <v>29</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>30</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>31</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>evol0330</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>33</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>34</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>35</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PERFA0261</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
         <v>37</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>38</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>39</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>GAG12103AR</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
         <v>41</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>42</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>43</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>TOR01522</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
         <v>45</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>46</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>47</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>logo-ferremax</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>49</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>50</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>51</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>login-bg</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
         <v>53</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>54</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>55</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>evol0330</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
         <v>57</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>58</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>59</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>evol3089</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
         <v>61</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>62</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>63</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>evol0025</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
         <v>65</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>66</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>67</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>evol3245</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
         <v>69</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>70</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>71</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>evol1970</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
         <v>73</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>74</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>75</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>evol115la</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
         <v>77</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>78</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>79</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>evo115tu</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
         <v>81</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>82</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>83</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>evol0028</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
         <v>85</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>86</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>87</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>evol3510</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>144</v>
+      </c>
+      <c r="B23" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>89</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>90</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>evorieg0153</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
         <v>92</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>93</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>94</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>evol0070</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
         <v>96</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>97</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>98</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>evol2530</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
         <v>100</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>101</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>102</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>evol0107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B27" t="s">
         <v>104</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>105</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>106</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>evol0435</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
         <v>108</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>109</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>110</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>evol0111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B29" t="s">
         <v>112</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>113</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>114</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>evol3970</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="B30" t="s">
         <v>116</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>117</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>118</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>evol0177</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B31" t="s">
         <v>120</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>121</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>122</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>evol0174</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>123</v>
+      </c>
+      <c r="B32" t="s">
+        <v>124</v>
+      </c>
+      <c r="C32" t="s">
+        <v>125</v>
+      </c>
+      <c r="D32" t="s">
+        <v>126</v>
+      </c>
+      <c r="E32" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>evol2205</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>127</v>
+      </c>
+      <c r="B33" t="s">
+        <v>128</v>
+      </c>
+      <c r="C33" t="s">
+        <v>129</v>
+      </c>
+      <c r="D33" t="s">
+        <v>130</v>
+      </c>
+      <c r="E33" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>evol1361</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>131</v>
+      </c>
+      <c r="B34" t="s">
+        <v>132</v>
+      </c>
+      <c r="C34" t="s">
+        <v>133</v>
+      </c>
+      <c r="D34" t="s">
+        <v>134</v>
+      </c>
+      <c r="E34" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>evol3210</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>135</v>
+      </c>
+      <c r="B35" t="s">
+        <v>136</v>
+      </c>
+      <c r="C35" t="s">
+        <v>137</v>
+      </c>
+      <c r="D35" t="s">
+        <v>138</v>
+      </c>
+      <c r="E35" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>evol5530</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>139</v>
+      </c>
+      <c r="B36" t="s">
+        <v>140</v>
+      </c>
+      <c r="C36" t="s">
+        <v>141</v>
+      </c>
+      <c r="D36" t="s">
+        <v>142</v>
+      </c>
+      <c r="E36" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>evo115co</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
subi img: GAG1685AR, GAG12301AR, ISAALAMF16, EA5310MT
</commit_message>
<xml_diff>
--- a/imagenes_drive.xlsx
+++ b/imagenes_drive.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,856 +458,944 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>EVOL0174.png</t>
+          <t>G1685AR.png</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1-YJjxDGKGERzcM6ZrMQdU8EXhrcWRnlt</t>
+          <t>1BEc5fw2mn1pWdTFtKCc1Ac5IPrCo3PFq</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1-YJjxDGKGERzcM6ZrMQdU8EXhrcWRnlt/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1BEc5fw2mn1pWdTFtKCc1Ac5IPrCo3PFq/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1-YJjxDGKGERzcM6ZrMQdU8EXhrcWRnlt</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1BEc5fw2mn1pWdTFtKCc1Ac5IPrCo3PFq</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>TF414.png</t>
+          <t>G12301AR-.png</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1KXEo3cSB5Aj_dPAW8X1-iG2eNGK4oNEr</t>
+          <t>1_UBXdXmyrPs0EwBnhV90mfhI3ZdSyn8H</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1KXEo3cSB5Aj_dPAW8X1-iG2eNGK4oNEr/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1_UBXdXmyrPs0EwBnhV90mfhI3ZdSyn8H/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1KXEo3cSB5Aj_dPAW8X1-iG2eNGK4oNEr</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1_UBXdXmyrPs0EwBnhV90mfhI3ZdSyn8H</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>evo115la.jpg</t>
+          <t>ISAALAMF16.png</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1xB_fFOvMWyAcqkpvUq7xMqq-iHuscSbd</t>
+          <t>14BogV6rHDIcL1bJzvKgItflTszBh2Yjx</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1xB_fFOvMWyAcqkpvUq7xMqq-iHuscSbd/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/14BogV6rHDIcL1bJzvKgItflTszBh2Yjx/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1xB_fFOvMWyAcqkpvUq7xMqq-iHuscSbd</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=14BogV6rHDIcL1bJzvKgItflTszBh2Yjx</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CON205.png</t>
+          <t>EA5310MT.png</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1LJxUYab9xJeV45iqUUz8RhH5UbnlycXa</t>
+          <t>168x1fBgYxstgD60EyOUekzYk21Cswij6</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1LJxUYab9xJeV45iqUUz8RhH5UbnlycXa/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/168x1fBgYxstgD60EyOUekzYk21Cswij6/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1LJxUYab9xJeV45iqUUz8RhH5UbnlycXa</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=168x1fBgYxstgD60EyOUekzYk21Cswij6</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ALI70.png</t>
+          <t>EVOL0174.png</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>118_Mew5CJz8YNrVjxiGgKooC9GHL40wA</t>
+          <t>1-YJjxDGKGERzcM6ZrMQdU8EXhrcWRnlt</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/118_Mew5CJz8YNrVjxiGgKooC9GHL40wA/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1-YJjxDGKGERzcM6ZrMQdU8EXhrcWRnlt/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=118_Mew5CJz8YNrVjxiGgKooC9GHL40wA</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1-YJjxDGKGERzcM6ZrMQdU8EXhrcWRnlt</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>SIM18310.png</t>
+          <t>TF414.png</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>13cioMVntBUSCdPldxG-2kDu8-KoWxIa5</t>
+          <t>1KXEo3cSB5Aj_dPAW8X1-iG2eNGK4oNEr</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/13cioMVntBUSCdPldxG-2kDu8-KoWxIa5/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1KXEo3cSB5Aj_dPAW8X1-iG2eNGK4oNEr/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=13cioMVntBUSCdPldxG-2kDu8-KoWxIa5</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1KXEo3cSB5Aj_dPAW8X1-iG2eNGK4oNEr</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>KIMERAC1.png</t>
+          <t>evo115la.jpg</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1hs0JvOUNyVuX5zfqUIACnXVADRBcgGiS</t>
+          <t>1xB_fFOvMWyAcqkpvUq7xMqq-iHuscSbd</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1hs0JvOUNyVuX5zfqUIACnXVADRBcgGiS/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1xB_fFOvMWyAcqkpvUq7xMqq-iHuscSbd/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1hs0JvOUNyVuX5zfqUIACnXVADRBcgGiS</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1xB_fFOvMWyAcqkpvUq7xMqq-iHuscSbd</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>PROBOT41.png</t>
+          <t>CON205.png</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1qrNWZscYLaNY3tjBvyWBCrhyf_YkY9P_</t>
+          <t>1LJxUYab9xJeV45iqUUz8RhH5UbnlycXa</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1qrNWZscYLaNY3tjBvyWBCrhyf_YkY9P_/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1LJxUYab9xJeV45iqUUz8RhH5UbnlycXa/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1qrNWZscYLaNY3tjBvyWBCrhyf_YkY9P_</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1LJxUYab9xJeV45iqUUz8RhH5UbnlycXa</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>evorieg0153.jpg</t>
+          <t>ALI70.png</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1lKfYjkIwKWP0ylRb7kAHB6MEsxMj5AyG</t>
+          <t>118_Mew5CJz8YNrVjxiGgKooC9GHL40wA</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1lKfYjkIwKWP0ylRb7kAHB6MEsxMj5AyG/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/118_Mew5CJz8YNrVjxiGgKooC9GHL40wA/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1lKfYjkIwKWP0ylRb7kAHB6MEsxMj5AyG</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=118_Mew5CJz8YNrVjxiGgKooC9GHL40wA</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>EGWX 01.png</t>
+          <t>SIM18310.png</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1BgwDF-x074YoMMB-mDYESEaqC2f_yOjJ</t>
+          <t>13cioMVntBUSCdPldxG-2kDu8-KoWxIa5</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1BgwDF-x074YoMMB-mDYESEaqC2f_yOjJ/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/13cioMVntBUSCdPldxG-2kDu8-KoWxIa5/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1BgwDF-x074YoMMB-mDYESEaqC2f_yOjJ</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=13cioMVntBUSCdPldxG-2kDu8-KoWxIa5</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>EGWX 02.png</t>
+          <t>KIMERAC1.png</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>1EDLSpqESmqhKp7xv2VUi5tJfPNY87I3H</t>
+          <t>1hs0JvOUNyVuX5zfqUIACnXVADRBcgGiS</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1EDLSpqESmqhKp7xv2VUi5tJfPNY87I3H/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1hs0JvOUNyVuX5zfqUIACnXVADRBcgGiS/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1EDLSpqESmqhKp7xv2VUi5tJfPNY87I3H</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1hs0JvOUNyVuX5zfqUIACnXVADRBcgGiS</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>PX120314.png</t>
+          <t>PROBOT41.png</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1weDOT_VWkZKZAz4jS8TVZsetiUcvCN9l</t>
+          <t>1qrNWZscYLaNY3tjBvyWBCrhyf_YkY9P_</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1weDOT_VWkZKZAz4jS8TVZsetiUcvCN9l/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1qrNWZscYLaNY3tjBvyWBCrhyf_YkY9P_/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1weDOT_VWkZKZAz4jS8TVZsetiUcvCN9l</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1qrNWZscYLaNY3tjBvyWBCrhyf_YkY9P_</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>evol0088.png</t>
+          <t>evorieg0153.jpg</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>1nfI5VLK3uGqGq2WeJTrgiggCfpxO2nW9</t>
+          <t>1lKfYjkIwKWP0ylRb7kAHB6MEsxMj5AyG</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1nfI5VLK3uGqGq2WeJTrgiggCfpxO2nW9/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1lKfYjkIwKWP0ylRb7kAHB6MEsxMj5AyG/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1nfI5VLK3uGqGq2WeJTrgiggCfpxO2nW9</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1lKfYjkIwKWP0ylRb7kAHB6MEsxMj5AyG</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>evol1000.png</t>
+          <t>EGWX 01.png</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>1LktIgDVrU9vZgoZ2NVNIvUR0nreN7E0k</t>
+          <t>1BgwDF-x074YoMMB-mDYESEaqC2f_yOjJ</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1LktIgDVrU9vZgoZ2NVNIvUR0nreN7E0k/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1BgwDF-x074YoMMB-mDYESEaqC2f_yOjJ/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1LktIgDVrU9vZgoZ2NVNIvUR0nreN7E0k</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1BgwDF-x074YoMMB-mDYESEaqC2f_yOjJ</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>evol0330.png</t>
+          <t>EGWX 02.png</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>1_woEN7ahCyphJcQooMGZU51SaSrhcw2H</t>
+          <t>1EDLSpqESmqhKp7xv2VUi5tJfPNY87I3H</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1_woEN7ahCyphJcQooMGZU51SaSrhcw2H/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1EDLSpqESmqhKp7xv2VUi5tJfPNY87I3H/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1_woEN7ahCyphJcQooMGZU51SaSrhcw2H</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1EDLSpqESmqhKp7xv2VUi5tJfPNY87I3H</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>GAG12103AR.jpg</t>
+          <t>PX120314.png</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>19PO9oKCI7tFYmwSmls9HncZeKFLKYsHM</t>
+          <t>1weDOT_VWkZKZAz4jS8TVZsetiUcvCN9l</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/19PO9oKCI7tFYmwSmls9HncZeKFLKYsHM/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1weDOT_VWkZKZAz4jS8TVZsetiUcvCN9l/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=19PO9oKCI7tFYmwSmls9HncZeKFLKYsHM</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1weDOT_VWkZKZAz4jS8TVZsetiUcvCN9l</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>TOR01522.jpg</t>
+          <t>evol0088.png</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>1D6zNN_9DGy0dFt9raoWvefgiUeE2dVYx</t>
+          <t>1nfI5VLK3uGqGq2WeJTrgiggCfpxO2nW9</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1D6zNN_9DGy0dFt9raoWvefgiUeE2dVYx/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1nfI5VLK3uGqGq2WeJTrgiggCfpxO2nW9/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1D6zNN_9DGy0dFt9raoWvefgiUeE2dVYx</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1nfI5VLK3uGqGq2WeJTrgiggCfpxO2nW9</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>logo-ferremax.png</t>
+          <t>evol1000.png</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>1QyHbyrm4L_XB5o-DT7UhtvcKO3P1PsQq</t>
+          <t>1LktIgDVrU9vZgoZ2NVNIvUR0nreN7E0k</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1QyHbyrm4L_XB5o-DT7UhtvcKO3P1PsQq/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1LktIgDVrU9vZgoZ2NVNIvUR0nreN7E0k/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1QyHbyrm4L_XB5o-DT7UhtvcKO3P1PsQq</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1LktIgDVrU9vZgoZ2NVNIvUR0nreN7E0k</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>login-bg.png</t>
+          <t>evol0330.png</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>1KK_TQrE0L6lVvyr8tfVlByktAqgtNhpn</t>
+          <t>1_woEN7ahCyphJcQooMGZU51SaSrhcw2H</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1KK_TQrE0L6lVvyr8tfVlByktAqgtNhpn/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1_woEN7ahCyphJcQooMGZU51SaSrhcw2H/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1KK_TQrE0L6lVvyr8tfVlByktAqgtNhpn</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1_woEN7ahCyphJcQooMGZU51SaSrhcw2H</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>evol0330.jpg</t>
+          <t>GAG12103AR.jpg</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>1p1QSEbeQl-dK5JE4QS99d5BD1VTBKT77</t>
+          <t>19PO9oKCI7tFYmwSmls9HncZeKFLKYsHM</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1p1QSEbeQl-dK5JE4QS99d5BD1VTBKT77/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/19PO9oKCI7tFYmwSmls9HncZeKFLKYsHM/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1p1QSEbeQl-dK5JE4QS99d5BD1VTBKT77</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=19PO9oKCI7tFYmwSmls9HncZeKFLKYsHM</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>evol3089.jpg</t>
+          <t>TOR01522.jpg</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>1Mzg3Z8QvvJabPNR36K7tFWAEeTY2U2Hw</t>
+          <t>1D6zNN_9DGy0dFt9raoWvefgiUeE2dVYx</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1Mzg3Z8QvvJabPNR36K7tFWAEeTY2U2Hw/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1D6zNN_9DGy0dFt9raoWvefgiUeE2dVYx/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1Mzg3Z8QvvJabPNR36K7tFWAEeTY2U2Hw</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1D6zNN_9DGy0dFt9raoWvefgiUeE2dVYx</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>evol0025.jpg</t>
+          <t>logo-ferremax.png</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>1iBM7F-xqNihiERpP73UQvQJE0kVFGJKO</t>
+          <t>1QyHbyrm4L_XB5o-DT7UhtvcKO3P1PsQq</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1iBM7F-xqNihiERpP73UQvQJE0kVFGJKO/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1QyHbyrm4L_XB5o-DT7UhtvcKO3P1PsQq/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1iBM7F-xqNihiERpP73UQvQJE0kVFGJKO</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1QyHbyrm4L_XB5o-DT7UhtvcKO3P1PsQq</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>evol3245.jpg</t>
+          <t>login-bg.png</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>1QQ8ZLm32-FoopDzdjhzc9MNivVFc7fLM</t>
+          <t>1KK_TQrE0L6lVvyr8tfVlByktAqgtNhpn</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1QQ8ZLm32-FoopDzdjhzc9MNivVFc7fLM/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1KK_TQrE0L6lVvyr8tfVlByktAqgtNhpn/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1QQ8ZLm32-FoopDzdjhzc9MNivVFc7fLM</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1KK_TQrE0L6lVvyr8tfVlByktAqgtNhpn</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>evol1970.jpg</t>
+          <t>evol0330.jpg</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>14IeVqqroYofkw5cy2sBlHAU3UcX2g6Sn</t>
+          <t>1p1QSEbeQl-dK5JE4QS99d5BD1VTBKT77</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/14IeVqqroYofkw5cy2sBlHAU3UcX2g6Sn/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1p1QSEbeQl-dK5JE4QS99d5BD1VTBKT77/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=14IeVqqroYofkw5cy2sBlHAU3UcX2g6Sn</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1p1QSEbeQl-dK5JE4QS99d5BD1VTBKT77</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>evo115tu.jpg</t>
+          <t>evol3089.jpg</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>1mr4rYfnhWS8bgSpPkkRNKY8S5CbHYA_g</t>
+          <t>1Mzg3Z8QvvJabPNR36K7tFWAEeTY2U2Hw</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1mr4rYfnhWS8bgSpPkkRNKY8S5CbHYA_g/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1Mzg3Z8QvvJabPNR36K7tFWAEeTY2U2Hw/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1mr4rYfnhWS8bgSpPkkRNKY8S5CbHYA_g</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1Mzg3Z8QvvJabPNR36K7tFWAEeTY2U2Hw</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>evol0028.jpg</t>
+          <t>evol0025.jpg</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>1yRGivdseZJU3_Jm-GwG-n--8hV2TchR7</t>
+          <t>1iBM7F-xqNihiERpP73UQvQJE0kVFGJKO</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1yRGivdseZJU3_Jm-GwG-n--8hV2TchR7/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1iBM7F-xqNihiERpP73UQvQJE0kVFGJKO/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1yRGivdseZJU3_Jm-GwG-n--8hV2TchR7</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1iBM7F-xqNihiERpP73UQvQJE0kVFGJKO</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>evol3510.jpg</t>
+          <t>evol3245.jpg</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>1dXUQ9WsxzAZey_wt6G2mS7N6Li-NJbSV</t>
+          <t>1QQ8ZLm32-FoopDzdjhzc9MNivVFc7fLM</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1dXUQ9WsxzAZey_wt6G2mS7N6Li-NJbSV/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1QQ8ZLm32-FoopDzdjhzc9MNivVFc7fLM/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1dXUQ9WsxzAZey_wt6G2mS7N6Li-NJbSV</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1QQ8ZLm32-FoopDzdjhzc9MNivVFc7fLM</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>evol0070.jpg</t>
+          <t>evol1970.jpg</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>1J-fMUEInSiroJxGr1U5gDTEMgeOmmmDZ</t>
+          <t>14IeVqqroYofkw5cy2sBlHAU3UcX2g6Sn</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1J-fMUEInSiroJxGr1U5gDTEMgeOmmmDZ/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/14IeVqqroYofkw5cy2sBlHAU3UcX2g6Sn/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1J-fMUEInSiroJxGr1U5gDTEMgeOmmmDZ</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=14IeVqqroYofkw5cy2sBlHAU3UcX2g6Sn</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>evol2530.jpg</t>
+          <t>evo115tu.jpg</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>18k2YQNWcz_1BYQNM6bONKlUxSYJrY-No</t>
+          <t>1mr4rYfnhWS8bgSpPkkRNKY8S5CbHYA_g</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/18k2YQNWcz_1BYQNM6bONKlUxSYJrY-No/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1mr4rYfnhWS8bgSpPkkRNKY8S5CbHYA_g/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=18k2YQNWcz_1BYQNM6bONKlUxSYJrY-No</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1mr4rYfnhWS8bgSpPkkRNKY8S5CbHYA_g</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>evol0107.jpg</t>
+          <t>evol0028.jpg</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>13lnno2tsyVhl9Bl6l3A1L-lgnfiZi5gV</t>
+          <t>1yRGivdseZJU3_Jm-GwG-n--8hV2TchR7</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/13lnno2tsyVhl9Bl6l3A1L-lgnfiZi5gV/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1yRGivdseZJU3_Jm-GwG-n--8hV2TchR7/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=13lnno2tsyVhl9Bl6l3A1L-lgnfiZi5gV</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1yRGivdseZJU3_Jm-GwG-n--8hV2TchR7</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>evol0435.jpg</t>
+          <t>evol3510.jpg</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>1ZRBZHzi8Mjue2G8UsgZBb35L-zTImn0x</t>
+          <t>1dXUQ9WsxzAZey_wt6G2mS7N6Li-NJbSV</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1ZRBZHzi8Mjue2G8UsgZBb35L-zTImn0x/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1dXUQ9WsxzAZey_wt6G2mS7N6Li-NJbSV/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1ZRBZHzi8Mjue2G8UsgZBb35L-zTImn0x</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1dXUQ9WsxzAZey_wt6G2mS7N6Li-NJbSV</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>evol0111.jpg</t>
+          <t>evol0070.jpg</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>18PywtpchMGSXpToC9emFelBbnkIO851b</t>
+          <t>1J-fMUEInSiroJxGr1U5gDTEMgeOmmmDZ</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/18PywtpchMGSXpToC9emFelBbnkIO851b/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1J-fMUEInSiroJxGr1U5gDTEMgeOmmmDZ/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=18PywtpchMGSXpToC9emFelBbnkIO851b</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1J-fMUEInSiroJxGr1U5gDTEMgeOmmmDZ</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>evol3970.jpg</t>
+          <t>evol2530.jpg</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>1Zj40lKbiQQn6MmKqrYPvwOoJ4Ao_hQls</t>
+          <t>18k2YQNWcz_1BYQNM6bONKlUxSYJrY-No</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1Zj40lKbiQQn6MmKqrYPvwOoJ4Ao_hQls/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/18k2YQNWcz_1BYQNM6bONKlUxSYJrY-No/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1Zj40lKbiQQn6MmKqrYPvwOoJ4Ao_hQls</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=18k2YQNWcz_1BYQNM6bONKlUxSYJrY-No</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>evol0177.jpg</t>
+          <t>evol0107.jpg</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>1pA1s9ukL2Ucya6RudnbtpvHAxufEyqNn</t>
+          <t>13lnno2tsyVhl9Bl6l3A1L-lgnfiZi5gV</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1pA1s9ukL2Ucya6RudnbtpvHAxufEyqNn/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/13lnno2tsyVhl9Bl6l3A1L-lgnfiZi5gV/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1pA1s9ukL2Ucya6RudnbtpvHAxufEyqNn</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=13lnno2tsyVhl9Bl6l3A1L-lgnfiZi5gV</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>evol2205.jpg</t>
+          <t>evol0435.jpg</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>18tyxWko2V2O-a8Ub1xpQ10ZRn8k2g9OK</t>
+          <t>1ZRBZHzi8Mjue2G8UsgZBb35L-zTImn0x</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/18tyxWko2V2O-a8Ub1xpQ10ZRn8k2g9OK/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1ZRBZHzi8Mjue2G8UsgZBb35L-zTImn0x/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=18tyxWko2V2O-a8Ub1xpQ10ZRn8k2g9OK</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1ZRBZHzi8Mjue2G8UsgZBb35L-zTImn0x</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>evol1361.jpg</t>
+          <t>evol0111.jpg</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>19gc2N8G72IxRFVn4NFzcK_QvqFIegmV8</t>
+          <t>18PywtpchMGSXpToC9emFelBbnkIO851b</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/19gc2N8G72IxRFVn4NFzcK_QvqFIegmV8/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/18PywtpchMGSXpToC9emFelBbnkIO851b/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=19gc2N8G72IxRFVn4NFzcK_QvqFIegmV8</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=18PywtpchMGSXpToC9emFelBbnkIO851b</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>evol3210.jpg</t>
+          <t>evol3970.jpg</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>1TArjaa7JzfoYKxuitLH3gEeurJie_XEr</t>
+          <t>1Zj40lKbiQQn6MmKqrYPvwOoJ4Ao_hQls</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1TArjaa7JzfoYKxuitLH3gEeurJie_XEr/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1Zj40lKbiQQn6MmKqrYPvwOoJ4Ao_hQls/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1TArjaa7JzfoYKxuitLH3gEeurJie_XEr</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1Zj40lKbiQQn6MmKqrYPvwOoJ4Ao_hQls</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>evol5530.jpg</t>
+          <t>evol0177.jpg</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>1RXomu2FAaptqak7anXGjSh0oKhGaZcnF</t>
+          <t>1pA1s9ukL2Ucya6RudnbtpvHAxufEyqNn</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1RXomu2FAaptqak7anXGjSh0oKhGaZcnF/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1pA1s9ukL2Ucya6RudnbtpvHAxufEyqNn/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1RXomu2FAaptqak7anXGjSh0oKhGaZcnF</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1pA1s9ukL2Ucya6RudnbtpvHAxufEyqNn</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
+          <t>evol2205.jpg</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>18tyxWko2V2O-a8Ub1xpQ10ZRn8k2g9OK</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/18tyxWko2V2O-a8Ub1xpQ10ZRn8k2g9OK/view?usp=drivesdk</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/uc?export=view&amp;id=18tyxWko2V2O-a8Ub1xpQ10ZRn8k2g9OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>evol1361.jpg</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>19gc2N8G72IxRFVn4NFzcK_QvqFIegmV8</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/19gc2N8G72IxRFVn4NFzcK_QvqFIegmV8/view?usp=drivesdk</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/uc?export=view&amp;id=19gc2N8G72IxRFVn4NFzcK_QvqFIegmV8</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>evol3210.jpg</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>1TArjaa7JzfoYKxuitLH3gEeurJie_XEr</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1TArjaa7JzfoYKxuitLH3gEeurJie_XEr/view?usp=drivesdk</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/uc?export=view&amp;id=1TArjaa7JzfoYKxuitLH3gEeurJie_XEr</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>evol5530.jpg</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>1RXomu2FAaptqak7anXGjSh0oKhGaZcnF</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/file/d/1RXomu2FAaptqak7anXGjSh0oKhGaZcnF/view?usp=drivesdk</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/uc?export=view&amp;id=1RXomu2FAaptqak7anXGjSh0oKhGaZcnF</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
           <t>evo115co.jpg</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="B44" t="inlineStr">
         <is>
           <t>1OFRhg3wSMFQ6TYNMMxMweX1JIEsXmKdY</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="C44" t="inlineStr">
         <is>
           <t>https://drive.google.com/file/d/1OFRhg3wSMFQ6TYNMMxMweX1JIEsXmKdY/view?usp=drivesdk</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
+      <c r="D44" t="inlineStr">
         <is>
           <t>https://drive.google.com/uc?export=view&amp;id=1OFRhg3wSMFQ6TYNMMxMweX1JIEsXmKdY</t>
         </is>

</xml_diff>

<commit_message>
Mejora en la extracción del nombre de archivo para la columna 'articulo'- Modificado el algoritmo para manejar casos especiales con múltiples puntos en el nombre- Ahora utiliza rfind('.') para preservar puntos internos como en 'TF.414.png'- Garantiza que nombres como 'TF.414.png' se conviertan correctamente en 'TF.414'
</commit_message>
<xml_diff>
--- a/imagenes_drive.xlsx
+++ b/imagenes_drive.xlsx
@@ -198,6 +198,9 @@
     <t>https://drive.google.com/uc?export=view&amp;id=1KXEo3cSB5Aj_dPAW8X1-iG2eNGK4oNEr</t>
   </si>
   <si>
+    <t>TF.414</t>
+  </si>
+  <si>
     <t>GAG1685AR.png</t>
   </si>
   <si>
@@ -781,9 +784,6 @@
   </si>
   <si>
     <t>evo115co</t>
-  </si>
-  <si>
-    <t>TF.414</t>
   </si>
 </sst>
 </file>
@@ -1148,11 +1148,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="21.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1355,670 +1356,670 @@
         <v>58</v>
       </c>
       <c r="E12" t="s">
-        <v>254</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D13" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D14" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E14" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C15" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D15" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E15" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D16" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E16" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B17" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C17" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D17" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E17" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B18" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C18" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D18" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E18" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B19" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C19" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D19" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B20" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C20" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D20" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E20" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B21" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C21" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D21" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E21" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B22" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C22" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D22" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E22" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B23" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C23" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D23" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E23" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B24" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C24" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D24" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E24" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B25" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C25" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D25" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E25" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B26" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C26" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D26" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E26" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B27" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C27" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D27" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E27" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B28" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C28" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D28" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E28" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B29" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C29" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D29" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E29" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B30" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C30" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D30" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E30" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B31" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C31" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D31" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E31" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B32" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C32" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D32" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E32" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B33" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C33" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D33" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E33" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B34" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C34" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D34" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E34" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B35" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C35" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D35" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E35" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B36" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C36" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D36" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E36" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B37" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C37" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D37" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E37" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B38" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C38" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D38" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E38" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B39" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C39" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D39" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E39" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B40" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C40" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D40" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E40" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B41" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C41" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D41" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E41" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B42" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C42" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D42" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E42" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B43" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C43" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D43" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E43" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B44" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C44" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D44" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E44" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B45" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C45" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D45" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E45" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B46" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C46" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D46" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E46" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B47" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C47" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D47" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E47" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B48" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C48" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D48" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E48" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B49" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C49" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D49" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E49" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B50" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C50" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D50" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E50" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B51" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C51" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D51" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E51" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reorganización completa de los estilos para mayor claridadMedia queries ordenados de mayor a menor tamaño de pantallaSelectores más específicos para dispositivos pequeños (usando html body para aumentar la especificidad)Uso consistente de !important en las propiedades críticasConfiguración explícita para cada breakpoint, asegurando que no haya {huecos} en la cobertura
</commit_message>
<xml_diff>
--- a/imagenes_drive.xlsx
+++ b/imagenes_drive.xlsx
@@ -463,567 +463,567 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>EVOL0011.png</t>
+          <t>EVOL3088.png</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1SQ4RO0DwgN6iB16qKKJW4nOKO-P-9AZ3</t>
+          <t>1eIiLw76jRpOSREMEBPIDpjFFqkxjchM2</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1SQ4RO0DwgN6iB16qKKJW4nOKO-P-9AZ3/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1eIiLw76jRpOSREMEBPIDpjFFqkxjchM2/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1SQ4RO0DwgN6iB16qKKJW4nOKO-P-9AZ3</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1eIiLw76jRpOSREMEBPIDpjFFqkxjchM2</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>EVOL0011</t>
+          <t>EVOL3088</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>EVOL0010.png</t>
+          <t>EVOL3087.png</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1GxnmEGjpuhLnIQTUrBPOHbaKsMVc8ztN</t>
+          <t>1po1vu4rn4nYzrCkc62BP4VTXYT0ECK8h</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1GxnmEGjpuhLnIQTUrBPOHbaKsMVc8ztN/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1po1vu4rn4nYzrCkc62BP4VTXYT0ECK8h/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1GxnmEGjpuhLnIQTUrBPOHbaKsMVc8ztN</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1po1vu4rn4nYzrCkc62BP4VTXYT0ECK8h</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>EVOL0010</t>
+          <t>EVOL3087</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>EVOL0009.png</t>
+          <t>EVOL3086.png</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>17ABzRsKQ-aAb7OOIy4gjt7EM2XOgeKi3</t>
+          <t>1BvURk9_AZvhv7bu5cU165dzxtk54lrfP</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/17ABzRsKQ-aAb7OOIy4gjt7EM2XOgeKi3/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1BvURk9_AZvhv7bu5cU165dzxtk54lrfP/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=17ABzRsKQ-aAb7OOIy4gjt7EM2XOgeKi3</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1BvURk9_AZvhv7bu5cU165dzxtk54lrfP</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>EVOL0009</t>
+          <t>EVOL3086</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>EVOL0008.png</t>
+          <t>EVOL3089.png</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1io205s0lr5DzUCVGViGbT2u_eoQJZb2C</t>
+          <t>1lkFpCsC8W2m3LUIiKnNyq5iQ5T4dSGWY</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1io205s0lr5DzUCVGViGbT2u_eoQJZb2C/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1lkFpCsC8W2m3LUIiKnNyq5iQ5T4dSGWY/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1io205s0lr5DzUCVGViGbT2u_eoQJZb2C</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1lkFpCsC8W2m3LUIiKnNyq5iQ5T4dSGWY</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>EVOL0008</t>
+          <t>EVOL3089</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>EVOL6765.jpg</t>
+          <t>EVOL0011.png</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>15gfbTSnSVxp3RepFCtm2oOGlz219oyZh</t>
+          <t>1SQ4RO0DwgN6iB16qKKJW4nOKO-P-9AZ3</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/15gfbTSnSVxp3RepFCtm2oOGlz219oyZh/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1SQ4RO0DwgN6iB16qKKJW4nOKO-P-9AZ3/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=15gfbTSnSVxp3RepFCtm2oOGlz219oyZh</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1SQ4RO0DwgN6iB16qKKJW4nOKO-P-9AZ3</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>EVOL6765</t>
+          <t>EVOL0011</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>EVOL6760.png</t>
+          <t>EVOL0010.png</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1vn8sI2ITt5XjGHLb23Z05vILv_DVLw05</t>
+          <t>1GxnmEGjpuhLnIQTUrBPOHbaKsMVc8ztN</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1vn8sI2ITt5XjGHLb23Z05vILv_DVLw05/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1GxnmEGjpuhLnIQTUrBPOHbaKsMVc8ztN/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1vn8sI2ITt5XjGHLb23Z05vILv_DVLw05</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1GxnmEGjpuhLnIQTUrBPOHbaKsMVc8ztN</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>EVOL6760</t>
+          <t>EVOL0010</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>EVOL6715.png</t>
+          <t>EVOL0009.png</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1SN4-JQEpjlD5Q-TDn2v5lNQ1hFyKVot1</t>
+          <t>17ABzRsKQ-aAb7OOIy4gjt7EM2XOgeKi3</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1SN4-JQEpjlD5Q-TDn2v5lNQ1hFyKVot1/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/17ABzRsKQ-aAb7OOIy4gjt7EM2XOgeKi3/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1SN4-JQEpjlD5Q-TDn2v5lNQ1hFyKVot1</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=17ABzRsKQ-aAb7OOIy4gjt7EM2XOgeKi3</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>EVOL6715</t>
+          <t>EVOL0009</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>EVOL6222.png</t>
+          <t>EVOL0008.png</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1O-xOhjMBTW4WINz5wsnhNFHCn5EnT0Ki</t>
+          <t>1io205s0lr5DzUCVGViGbT2u_eoQJZb2C</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1O-xOhjMBTW4WINz5wsnhNFHCn5EnT0Ki/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1io205s0lr5DzUCVGViGbT2u_eoQJZb2C/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1O-xOhjMBTW4WINz5wsnhNFHCn5EnT0Ki</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1io205s0lr5DzUCVGViGbT2u_eoQJZb2C</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>EVOL6222</t>
+          <t>EVOL0008</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>EVOL6221.png</t>
+          <t>EVOL6765.jpg</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>19iuIRdeE_RammaNztz1KygdNq1tGTL8C</t>
+          <t>15gfbTSnSVxp3RepFCtm2oOGlz219oyZh</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/19iuIRdeE_RammaNztz1KygdNq1tGTL8C/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/15gfbTSnSVxp3RepFCtm2oOGlz219oyZh/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=19iuIRdeE_RammaNztz1KygdNq1tGTL8C</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=15gfbTSnSVxp3RepFCtm2oOGlz219oyZh</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>EVOL6221</t>
+          <t>EVOL6765</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>EVOL6210.png</t>
+          <t>EVOL6760.png</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>15mNv1wWkmsHpiLiWlg8jgv5yQVZt4Z1l</t>
+          <t>1vn8sI2ITt5XjGHLb23Z05vILv_DVLw05</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/15mNv1wWkmsHpiLiWlg8jgv5yQVZt4Z1l/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1vn8sI2ITt5XjGHLb23Z05vILv_DVLw05/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=15mNv1wWkmsHpiLiWlg8jgv5yQVZt4Z1l</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1vn8sI2ITt5XjGHLb23Z05vILv_DVLw05</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>EVOL6210</t>
+          <t>EVOL6760</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>EVOL6205.png</t>
+          <t>EVOL6715.png</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>11hBmjH-q6kh0_CNOGWTw6LnsXjbves0f</t>
+          <t>1SN4-JQEpjlD5Q-TDn2v5lNQ1hFyKVot1</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/11hBmjH-q6kh0_CNOGWTw6LnsXjbves0f/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1SN4-JQEpjlD5Q-TDn2v5lNQ1hFyKVot1/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=11hBmjH-q6kh0_CNOGWTw6LnsXjbves0f</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1SN4-JQEpjlD5Q-TDn2v5lNQ1hFyKVot1</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>EVOL6205</t>
+          <t>EVOL6715</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>EVOL3957.png</t>
+          <t>EVOL6222.png</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>14c8KBXNh6nrKA5S4u67BmU7nOAZL4Adk</t>
+          <t>1O-xOhjMBTW4WINz5wsnhNFHCn5EnT0Ki</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/14c8KBXNh6nrKA5S4u67BmU7nOAZL4Adk/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1O-xOhjMBTW4WINz5wsnhNFHCn5EnT0Ki/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=14c8KBXNh6nrKA5S4u67BmU7nOAZL4Adk</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1O-xOhjMBTW4WINz5wsnhNFHCn5EnT0Ki</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>EVOL3957</t>
+          <t>EVOL6222</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>EVOL3953.png</t>
+          <t>EVOL6221.png</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>1PWg5nUjF3Lzsf6MSF9eUD0K364TAsO1O</t>
+          <t>19iuIRdeE_RammaNztz1KygdNq1tGTL8C</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1PWg5nUjF3Lzsf6MSF9eUD0K364TAsO1O/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/19iuIRdeE_RammaNztz1KygdNq1tGTL8C/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1PWg5nUjF3Lzsf6MSF9eUD0K364TAsO1O</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=19iuIRdeE_RammaNztz1KygdNq1tGTL8C</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>EVOL3953</t>
+          <t>EVOL6221</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>EVOL3959.png</t>
+          <t>EVOL6210.png</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>1MtgmhF4llFOz-8-Kg3Xk0eOPlIrE6NqZ</t>
+          <t>15mNv1wWkmsHpiLiWlg8jgv5yQVZt4Z1l</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1MtgmhF4llFOz-8-Kg3Xk0eOPlIrE6NqZ/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/15mNv1wWkmsHpiLiWlg8jgv5yQVZt4Z1l/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1MtgmhF4llFOz-8-Kg3Xk0eOPlIrE6NqZ</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=15mNv1wWkmsHpiLiWlg8jgv5yQVZt4Z1l</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>EVOL3959</t>
+          <t>EVOL6210</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>EVOL3955.png</t>
+          <t>EVOL6205.png</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>1sRu-iyXG_A4UpHTtmWy4m_O-1eVKvO-f</t>
+          <t>11hBmjH-q6kh0_CNOGWTw6LnsXjbves0f</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1sRu-iyXG_A4UpHTtmWy4m_O-1eVKvO-f/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/11hBmjH-q6kh0_CNOGWTw6LnsXjbves0f/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1sRu-iyXG_A4UpHTtmWy4m_O-1eVKvO-f</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=11hBmjH-q6kh0_CNOGWTw6LnsXjbves0f</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>EVOL3955</t>
+          <t>EVOL6205</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>EVOL3961.png</t>
+          <t>EVOL3957.png</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>1h2_X5ZaWr3LDrgj_YErdS25QazR7X0od</t>
+          <t>14c8KBXNh6nrKA5S4u67BmU7nOAZL4Adk</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1h2_X5ZaWr3LDrgj_YErdS25QazR7X0od/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/14c8KBXNh6nrKA5S4u67BmU7nOAZL4Adk/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1h2_X5ZaWr3LDrgj_YErdS25QazR7X0od</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=14c8KBXNh6nrKA5S4u67BmU7nOAZL4Adk</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>EVOL3961</t>
+          <t>EVOL3957</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>EVOL0440.png</t>
+          <t>EVOL3953.png</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>1Ms54HbfpRLBZCKT8PoD-2ajd7x6LXc-z</t>
+          <t>1PWg5nUjF3Lzsf6MSF9eUD0K364TAsO1O</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1Ms54HbfpRLBZCKT8PoD-2ajd7x6LXc-z/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1PWg5nUjF3Lzsf6MSF9eUD0K364TAsO1O/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1Ms54HbfpRLBZCKT8PoD-2ajd7x6LXc-z</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1PWg5nUjF3Lzsf6MSF9eUD0K364TAsO1O</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>EVOL0440</t>
+          <t>EVOL3953</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>EVOL3088.png</t>
+          <t>EVOL3959.png</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>1Sg_TcDl02yfg5ci4N_aUxhguTMsJK1oS</t>
+          <t>1MtgmhF4llFOz-8-Kg3Xk0eOPlIrE6NqZ</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1Sg_TcDl02yfg5ci4N_aUxhguTMsJK1oS/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1MtgmhF4llFOz-8-Kg3Xk0eOPlIrE6NqZ/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1Sg_TcDl02yfg5ci4N_aUxhguTMsJK1oS</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1MtgmhF4llFOz-8-Kg3Xk0eOPlIrE6NqZ</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>EVOL3088</t>
+          <t>EVOL3959</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>EVOL3087.png</t>
+          <t>EVOL3955.png</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>1BtaWjX91R2Jb9m7lIR25yIc3K0bUFXh4</t>
+          <t>1sRu-iyXG_A4UpHTtmWy4m_O-1eVKvO-f</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1BtaWjX91R2Jb9m7lIR25yIc3K0bUFXh4/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1sRu-iyXG_A4UpHTtmWy4m_O-1eVKvO-f/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1BtaWjX91R2Jb9m7lIR25yIc3K0bUFXh4</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1sRu-iyXG_A4UpHTtmWy4m_O-1eVKvO-f</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>EVOL3087</t>
+          <t>EVOL3955</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>EVOL3086.png</t>
+          <t>EVOL3961.png</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>1cPh9vY23LMIJ6gxryWrzINzAnbU55Mpd</t>
+          <t>1h2_X5ZaWr3LDrgj_YErdS25QazR7X0od</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1cPh9vY23LMIJ6gxryWrzINzAnbU55Mpd/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1h2_X5ZaWr3LDrgj_YErdS25QazR7X0od/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1cPh9vY23LMIJ6gxryWrzINzAnbU55Mpd</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1h2_X5ZaWr3LDrgj_YErdS25QazR7X0od</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>EVOL3086</t>
+          <t>EVOL3961</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>EVOL3089.png</t>
+          <t>EVOL0440.png</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>1FxoJjxKuGkKQkyduEClxlKKO4PiTc2zI</t>
+          <t>1Ms54HbfpRLBZCKT8PoD-2ajd7x6LXc-z</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>https://drive.google.com/file/d/1FxoJjxKuGkKQkyduEClxlKKO4PiTc2zI/view?usp=drivesdk</t>
+          <t>https://drive.google.com/file/d/1Ms54HbfpRLBZCKT8PoD-2ajd7x6LXc-z/view?usp=drivesdk</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=view&amp;id=1FxoJjxKuGkKQkyduEClxlKKO4PiTc2zI</t>
+          <t>https://drive.google.com/uc?export=view&amp;id=1Ms54HbfpRLBZCKT8PoD-2ajd7x6LXc-z</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>EVOL3089</t>
+          <t>EVOL0440</t>
         </is>
       </c>
     </row>

</xml_diff>